<commit_message>
Worked on iakov i bratia
</commit_message>
<xml_diff>
--- a/integrator/test/Proba32.xlsx
+++ b/integrator/test/Proba32.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="761">
   <si>
     <t xml:space="preserve">1/W168a14</t>
   </si>
@@ -2217,34 +2217,34 @@
     <t xml:space="preserve">оуть сꙗ ꙗко-</t>
   </si>
   <si>
+    <t xml:space="preserve">περὶ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">περί </t>
+  </si>
+  <si>
+    <t xml:space="preserve">περί + Acc. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">οἱ περὶ Ἰάκωβον</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38/181a20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">въ  братꙗ его•</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ἰάκωβον</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ἰάκωβος</t>
+  </si>
+  <si>
+    <t xml:space="preserve">братꙗ</t>
+  </si>
+  <si>
     <t xml:space="preserve">аковъ  братꙗ го</t>
-  </si>
-  <si>
-    <t xml:space="preserve">περὶ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">περί </t>
-  </si>
-  <si>
-    <t xml:space="preserve">περί + Acc. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">οἱ περὶ Ἰάκωβον</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38/181a20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">въ  братꙗ его•</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ἰάκωβον</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ἰάκωβος</t>
-  </si>
-  <si>
-    <t xml:space="preserve">братꙗ</t>
   </si>
   <si>
     <t xml:space="preserve">его•</t>
@@ -3667,6 +3667,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="56" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3676,10 +3680,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="32" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3787,11 +3787,11 @@
   </sheetPr>
   <dimension ref="A1:AA204"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A63" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J76" activeCellId="0" sqref="J76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A161" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J183" activeCellId="0" sqref="J183"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="17.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14"/>
@@ -3801,7 +3801,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="5.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="12.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="10.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="10.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="8.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="6.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.22"/>
@@ -3815,7 +3815,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="6.22"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E4" s="5" t="s">
         <v>19</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E5" s="5" t="s">
         <v>25</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E6" s="12" t="s">
         <v>27</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="12" t="s">
         <v>27</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="12" t="s">
         <v>27</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E9" s="12" t="s">
         <v>37</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="14" t="s">
         <v>43</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E11" s="14" t="s">
         <v>49</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E12" s="5" t="s">
         <v>52</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E13" s="5" t="s">
         <v>60</v>
       </c>
@@ -4102,7 +4102,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="5" t="s">
         <v>63</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E15" s="5" t="s">
         <v>67</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="5" t="s">
         <v>74</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E17" s="5" t="s">
         <v>80</v>
       </c>
@@ -4204,7 +4204,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="5" t="s">
         <v>89</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="5" t="s">
         <v>80</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="5" t="s">
         <v>97</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="5" t="s">
         <v>97</v>
       </c>
@@ -4295,7 +4295,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="5" t="s">
         <v>97</v>
       </c>
@@ -4309,7 +4309,7 @@
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
     </row>
-    <row r="23" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="5"/>
       <c r="F23" s="11"/>
       <c r="G23" s="7"/>
@@ -4317,7 +4317,7 @@
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
     </row>
-    <row r="24" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="5" t="s">
         <v>106</v>
       </c>
@@ -4337,7 +4337,7 @@
       <c r="O24" s="25"/>
       <c r="Q24" s="26"/>
     </row>
-    <row r="25" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E25" s="5" t="s">
         <v>106</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="5"/>
       <c r="F26" s="11"/>
       <c r="G26" s="7"/>
@@ -4372,7 +4372,7 @@
       <c r="M26" s="9"/>
       <c r="Q26" s="21"/>
     </row>
-    <row r="27" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="5" t="s">
         <v>114</v>
       </c>
@@ -4391,7 +4391,7 @@
       </c>
       <c r="O27" s="25"/>
     </row>
-    <row r="28" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E28" s="5" t="s">
         <v>114</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="28"/>
       <c r="B29" s="8"/>
       <c r="C29" s="2"/>
@@ -4426,7 +4426,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="9"/>
     </row>
-    <row r="30" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E30" s="5" t="s">
         <v>121</v>
       </c>
@@ -4446,7 +4446,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="5" t="s">
         <v>121</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E32" s="5"/>
       <c r="F32" s="11"/>
       <c r="G32" s="7"/>
@@ -4474,7 +4474,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="9"/>
     </row>
-    <row r="33" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="5" t="s">
         <v>131</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E34" s="5" t="s">
         <v>137</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E35" s="5" t="s">
         <v>137</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="5" t="s">
         <v>147</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E37" s="5"/>
       <c r="F37" s="11"/>
       <c r="G37" s="7"/>
@@ -4562,7 +4562,7 @@
       <c r="L37" s="3"/>
       <c r="M37" s="9"/>
     </row>
-    <row r="38" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="28" t="s">
         <v>153</v>
       </c>
@@ -4593,7 +4593,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="28" t="s">
         <v>161</v>
       </c>
@@ -4617,7 +4617,7 @@
       <c r="L39" s="3"/>
       <c r="M39" s="9"/>
     </row>
-    <row r="40" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="28"/>
       <c r="B40" s="8"/>
       <c r="C40" s="2"/>
@@ -4641,7 +4641,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="28"/>
       <c r="B41" s="8"/>
       <c r="C41" s="2"/>
@@ -4665,7 +4665,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E42" s="5" t="s">
         <v>173</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E43" s="5" t="s">
         <v>176</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E44" s="5" t="s">
         <v>176</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E45" s="5" t="s">
         <v>183</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E46" s="5" t="s">
         <v>184</v>
       </c>
@@ -4768,7 +4768,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="28" t="s">
         <v>187</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
         <v>198</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
         <v>205</v>
       </c>
@@ -4860,7 +4860,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="28" t="s">
         <v>209</v>
       </c>
@@ -4888,7 +4888,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E52" s="5" t="s">
         <v>217</v>
       </c>
@@ -4908,7 +4908,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="28" t="s">
         <v>222</v>
       </c>
@@ -4936,7 +4936,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
         <v>226</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="28" t="s">
         <v>232</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E56" s="5" t="s">
         <v>237</v>
       </c>
@@ -5012,7 +5012,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E57" s="5" t="s">
         <v>242</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E58" s="5" t="s">
         <v>248</v>
       </c>
@@ -5052,7 +5052,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E59" s="5" t="s">
         <v>237</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E60" s="5" t="s">
         <v>237</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E61" s="5" t="s">
         <v>237</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E62" s="5" t="s">
         <v>237</v>
       </c>
@@ -5132,7 +5132,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="5" t="s">
         <v>237</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E64" s="5" t="s">
         <v>237</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2"/>
       <c r="B65" s="31"/>
       <c r="C65" s="2"/>
@@ -5198,7 +5198,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="18" t="s">
         <v>269</v>
       </c>
@@ -5260,7 +5260,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="17"/>
       <c r="D69" s="40"/>
       <c r="E69" s="14" t="s">
@@ -5285,7 +5285,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E70" s="14" t="s">
         <v>279</v>
       </c>
@@ -5314,7 +5314,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E71" s="14" t="s">
         <v>279</v>
       </c>
@@ -5343,7 +5343,7 @@
       </c>
       <c r="R71" s="33"/>
     </row>
-    <row r="72" customFormat="false" ht="34.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="47" t="s">
         <v>291</v>
       </c>
@@ -5378,7 +5378,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="34.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="47" t="s">
         <v>301</v>
       </c>
@@ -5406,10 +5406,10 @@
       <c r="M73" s="53"/>
       <c r="Q73" s="30"/>
     </row>
-    <row r="74" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q74" s="56"/>
     </row>
-    <row r="75" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2"/>
       <c r="B75" s="31"/>
       <c r="C75" s="2"/>
@@ -5435,7 +5435,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="18" t="s">
         <v>269</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="78" s="60" customFormat="true" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" s="60" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="57"/>
       <c r="B78" s="57"/>
       <c r="C78" s="57"/>
@@ -5496,7 +5496,7 @@
       <c r="N78" s="59"/>
       <c r="R78" s="61"/>
     </row>
-    <row r="79" s="60" customFormat="true" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" s="60" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="11" t="s">
         <v>314</v>
       </c>
@@ -5527,7 +5527,7 @@
       <c r="N79" s="59"/>
       <c r="R79" s="61"/>
     </row>
-    <row r="80" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2"/>
       <c r="E80" s="59"/>
       <c r="F80" s="63"/>
@@ -5536,7 +5536,7 @@
       <c r="I80" s="63"/>
       <c r="J80" s="63"/>
     </row>
-    <row r="81" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="64"/>
       <c r="B81" s="64"/>
       <c r="C81" s="64"/>
@@ -5564,7 +5564,7 @@
       </c>
       <c r="N81" s="69"/>
     </row>
-    <row r="82" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E82" s="65" t="s">
         <v>322</v>
       </c>
@@ -5590,7 +5590,7 @@
       </c>
       <c r="N82" s="69"/>
     </row>
-    <row r="83" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="28"/>
       <c r="B83" s="8"/>
       <c r="C83" s="2"/>
@@ -5617,7 +5617,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E84" s="5" t="s">
         <v>334</v>
       </c>
@@ -5640,7 +5640,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="28" t="s">
         <v>340</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="73" t="s">
         <v>348</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E87" s="5" t="s">
         <v>354</v>
       </c>
@@ -5725,7 +5725,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="28" t="s">
         <v>360</v>
       </c>
@@ -5759,7 +5759,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="63" t="s">
         <v>370</v>
       </c>
@@ -5788,7 +5788,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E90" s="5" t="s">
         <v>376</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E91" s="5" t="s">
         <v>381</v>
       </c>
@@ -5831,7 +5831,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E92" s="5"/>
       <c r="F92" s="11" t="s">
         <v>179</v>
@@ -5850,7 +5850,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E93" s="5" t="s">
         <v>390</v>
       </c>
@@ -5869,8 +5869,9 @@
       <c r="M93" s="9" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="94" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T93" s="0"/>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E94" s="5"/>
       <c r="F94" s="11" t="s">
         <v>179</v>
@@ -5888,8 +5889,9 @@
       <c r="N94" s="3" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="95" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T94" s="0"/>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="28" t="s">
         <v>397</v>
       </c>
@@ -5916,8 +5918,9 @@
       <c r="M95" s="9" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="96" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T95" s="0"/>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="28"/>
       <c r="B96" s="8"/>
       <c r="C96" s="2"/>
@@ -5940,8 +5943,9 @@
       <c r="M96" s="9" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="97" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T96" s="0"/>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="28" t="s">
         <v>397</v>
       </c>
@@ -5968,8 +5972,9 @@
       <c r="M97" s="9" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="98" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T97" s="0"/>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="28" t="s">
         <v>401</v>
       </c>
@@ -5997,8 +6002,9 @@
       <c r="N98" s="3" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="99" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T98" s="0"/>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="18" t="s">
         <v>406</v>
       </c>
@@ -6028,8 +6034,9 @@
       <c r="M99" s="52" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="100" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T99" s="0"/>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E100" s="18" t="s">
         <v>412</v>
       </c>
@@ -6051,8 +6058,9 @@
       <c r="M100" s="20" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="101" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T100" s="0"/>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E101" s="18" t="s">
         <v>415</v>
       </c>
@@ -6074,8 +6082,9 @@
       <c r="M101" s="75" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="102" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T101" s="0"/>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="18" t="s">
         <v>420</v>
       </c>
@@ -6105,8 +6114,9 @@
       <c r="M102" s="76" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="103" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T102" s="0"/>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="18" t="s">
         <v>427</v>
       </c>
@@ -6136,8 +6146,9 @@
       <c r="M103" s="76" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="104" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T103" s="0"/>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="18" t="s">
         <v>429</v>
       </c>
@@ -6167,8 +6178,9 @@
       <c r="M104" s="76" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="105" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T104" s="0"/>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="18" t="s">
         <v>429</v>
       </c>
@@ -6196,8 +6208,9 @@
       <c r="M105" s="76" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="106" s="77" customFormat="true" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T105" s="0"/>
+    </row>
+    <row r="106" s="77" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="17"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
@@ -6227,18 +6240,16 @@
       <c r="P106" s="3"/>
       <c r="Q106" s="3"/>
       <c r="R106" s="9"/>
-      <c r="T106" s="78"/>
-      <c r="U106" s="78"/>
-      <c r="V106" s="78"/>
-      <c r="W106" s="78"/>
-      <c r="X106" s="78"/>
-      <c r="Y106" s="78" t="s">
-        <v>442</v>
-      </c>
-      <c r="Z106" s="78"/>
+      <c r="T106" s="0"/>
+      <c r="U106" s="0"/>
+      <c r="V106" s="0"/>
+      <c r="W106" s="0"/>
+      <c r="X106" s="0"/>
+      <c r="Y106" s="0"/>
+      <c r="Z106" s="0"/>
       <c r="AA106" s="78"/>
     </row>
-    <row r="107" s="77" customFormat="true" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" s="77" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="18" t="s">
         <v>443</v>
       </c>
@@ -6273,18 +6284,16 @@
       <c r="P107" s="3"/>
       <c r="Q107" s="3"/>
       <c r="R107" s="9"/>
-      <c r="T107" s="78"/>
-      <c r="U107" s="78"/>
-      <c r="V107" s="78"/>
-      <c r="W107" s="78"/>
-      <c r="X107" s="78"/>
-      <c r="Y107" s="78" t="s">
-        <v>448</v>
-      </c>
-      <c r="Z107" s="78"/>
+      <c r="T107" s="0"/>
+      <c r="U107" s="0"/>
+      <c r="V107" s="0"/>
+      <c r="W107" s="0"/>
+      <c r="X107" s="0"/>
+      <c r="Y107" s="0"/>
+      <c r="Z107" s="0"/>
       <c r="AA107" s="78"/>
     </row>
-    <row r="108" s="77" customFormat="true" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" s="77" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="18" t="s">
         <v>449</v>
       </c>
@@ -6319,16 +6328,16 @@
       <c r="P108" s="3"/>
       <c r="Q108" s="3"/>
       <c r="R108" s="9"/>
-      <c r="T108" s="78"/>
-      <c r="U108" s="78"/>
-      <c r="V108" s="78"/>
-      <c r="W108" s="78"/>
-      <c r="X108" s="78"/>
-      <c r="Y108" s="78"/>
-      <c r="Z108" s="78"/>
+      <c r="T108" s="0"/>
+      <c r="U108" s="0"/>
+      <c r="V108" s="0"/>
+      <c r="W108" s="0"/>
+      <c r="X108" s="0"/>
+      <c r="Y108" s="0"/>
+      <c r="Z108" s="0"/>
       <c r="AA108" s="78"/>
     </row>
-    <row r="109" s="77" customFormat="true" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" s="77" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="17"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
@@ -6358,18 +6367,16 @@
       <c r="P109" s="3"/>
       <c r="Q109" s="3"/>
       <c r="R109" s="9"/>
-      <c r="T109" s="78"/>
-      <c r="U109" s="78"/>
-      <c r="V109" s="78"/>
-      <c r="W109" s="78"/>
-      <c r="X109" s="78"/>
-      <c r="Y109" s="78" t="s">
-        <v>456</v>
-      </c>
-      <c r="Z109" s="78"/>
+      <c r="T109" s="0"/>
+      <c r="U109" s="0"/>
+      <c r="V109" s="0"/>
+      <c r="W109" s="0"/>
+      <c r="X109" s="0"/>
+      <c r="Y109" s="0"/>
+      <c r="Z109" s="0"/>
       <c r="AA109" s="78"/>
     </row>
-    <row r="110" s="77" customFormat="true" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" s="77" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="18" t="s">
         <v>457</v>
       </c>
@@ -6404,18 +6411,16 @@
       <c r="P110" s="3"/>
       <c r="Q110" s="3"/>
       <c r="R110" s="9"/>
-      <c r="T110" s="78"/>
-      <c r="U110" s="78"/>
-      <c r="V110" s="78"/>
-      <c r="W110" s="78"/>
-      <c r="X110" s="78"/>
-      <c r="Y110" s="78" t="s">
-        <v>461</v>
-      </c>
-      <c r="Z110" s="78"/>
+      <c r="T110" s="0"/>
+      <c r="U110" s="0"/>
+      <c r="V110" s="0"/>
+      <c r="W110" s="0"/>
+      <c r="X110" s="0"/>
+      <c r="Y110" s="0"/>
+      <c r="Z110" s="0"/>
       <c r="AA110" s="78"/>
     </row>
-    <row r="111" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="77"/>
       <c r="B111" s="17"/>
       <c r="C111" s="2"/>
@@ -6441,8 +6446,9 @@
       <c r="M111" s="76" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="112" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T111" s="0"/>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="77"/>
       <c r="B112" s="17"/>
       <c r="C112" s="2"/>
@@ -6471,8 +6477,9 @@
         <v>160</v>
       </c>
       <c r="N112" s="80"/>
-    </row>
-    <row r="113" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T112" s="0"/>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="77"/>
       <c r="B113" s="17"/>
       <c r="C113" s="2"/>
@@ -6494,8 +6501,9 @@
       <c r="K113" s="18"/>
       <c r="L113" s="77"/>
       <c r="M113" s="76"/>
-    </row>
-    <row r="114" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T113" s="0"/>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="77"/>
       <c r="B114" s="17"/>
       <c r="C114" s="2"/>
@@ -6522,7 +6530,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="77"/>
       <c r="B115" s="17"/>
       <c r="C115" s="2"/>
@@ -6549,7 +6557,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="77"/>
       <c r="B116" s="17"/>
       <c r="C116" s="2"/>
@@ -6576,7 +6584,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="77"/>
       <c r="B117" s="17"/>
       <c r="C117" s="2"/>
@@ -6603,7 +6611,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="77"/>
       <c r="B118" s="17"/>
       <c r="C118" s="2"/>
@@ -6630,7 +6638,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="20" t="s">
         <v>484</v>
       </c>
@@ -6663,7 +6671,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E121" s="20"/>
       <c r="F121" s="11"/>
       <c r="G121" s="16"/>
@@ -6684,7 +6692,7 @@
       </c>
       <c r="S121" s="85"/>
     </row>
-    <row r="122" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="18" t="s">
         <v>491</v>
       </c>
@@ -6720,7 +6728,7 @@
       <c r="S122" s="88"/>
       <c r="T122" s="88"/>
     </row>
-    <row r="123" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="14" t="s">
         <v>498</v>
       </c>
@@ -6760,7 +6768,7 @@
       <c r="S123" s="88"/>
       <c r="T123" s="88"/>
     </row>
-    <row r="124" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="88"/>
       <c r="B124" s="88"/>
       <c r="C124" s="88"/>
@@ -6796,7 +6804,7 @@
       <c r="S124" s="88"/>
       <c r="T124" s="88"/>
     </row>
-    <row r="125" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="88"/>
       <c r="B125" s="88"/>
       <c r="C125" s="88"/>
@@ -6834,7 +6842,7 @@
       <c r="S125" s="88"/>
       <c r="T125" s="88"/>
     </row>
-    <row r="126" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="88"/>
       <c r="B126" s="88"/>
       <c r="C126" s="88"/>
@@ -6872,7 +6880,7 @@
       <c r="S126" s="88"/>
       <c r="T126" s="88"/>
     </row>
-    <row r="127" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="88"/>
       <c r="B127" s="88"/>
       <c r="C127" s="88"/>
@@ -6885,7 +6893,7 @@
       <c r="S127" s="88"/>
       <c r="T127" s="88"/>
     </row>
-    <row r="128" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="88"/>
       <c r="B128" s="88"/>
       <c r="C128" s="88"/>
@@ -6921,7 +6929,7 @@
       <c r="S128" s="14"/>
       <c r="T128" s="101"/>
     </row>
-    <row r="129" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="88"/>
       <c r="B129" s="88"/>
       <c r="C129" s="88"/>
@@ -6954,7 +6962,7 @@
       <c r="S129" s="88"/>
       <c r="T129" s="88"/>
     </row>
-    <row r="130" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="88"/>
       <c r="B130" s="88"/>
       <c r="C130" s="88"/>
@@ -6983,7 +6991,7 @@
       <c r="S130" s="88"/>
       <c r="T130" s="88"/>
     </row>
-    <row r="131" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="88"/>
       <c r="B131" s="88"/>
       <c r="C131" s="88"/>
@@ -7008,7 +7016,7 @@
       <c r="S131" s="88"/>
       <c r="T131" s="88"/>
     </row>
-    <row r="132" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="88"/>
       <c r="B132" s="88"/>
       <c r="C132" s="88"/>
@@ -7046,7 +7054,7 @@
       <c r="S132" s="88"/>
       <c r="T132" s="88"/>
     </row>
-    <row r="133" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="88"/>
       <c r="B133" s="88"/>
       <c r="C133" s="88"/>
@@ -7084,7 +7092,7 @@
       <c r="S133" s="88"/>
       <c r="T133" s="88"/>
     </row>
-    <row r="134" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="88"/>
       <c r="B134" s="88"/>
       <c r="C134" s="88"/>
@@ -7122,7 +7130,7 @@
       <c r="S134" s="88"/>
       <c r="T134" s="88"/>
     </row>
-    <row r="135" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="18" t="s">
         <v>547</v>
       </c>
@@ -7164,7 +7172,7 @@
       <c r="S135" s="88"/>
       <c r="T135" s="88"/>
     </row>
-    <row r="136" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="88"/>
       <c r="B136" s="88"/>
       <c r="C136" s="88"/>
@@ -7204,7 +7212,7 @@
       <c r="S136" s="88"/>
       <c r="T136" s="88"/>
     </row>
-    <row r="137" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="88"/>
       <c r="B137" s="88"/>
       <c r="C137" s="88"/>
@@ -7236,7 +7244,7 @@
       <c r="S137" s="88"/>
       <c r="T137" s="88"/>
     </row>
-    <row r="138" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="88"/>
       <c r="B138" s="88"/>
       <c r="C138" s="88"/>
@@ -7266,7 +7274,7 @@
       <c r="S138" s="88"/>
       <c r="T138" s="88"/>
     </row>
-    <row r="139" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="88"/>
       <c r="B139" s="88"/>
       <c r="C139" s="88"/>
@@ -7279,7 +7287,7 @@
       <c r="S139" s="88"/>
       <c r="T139" s="88"/>
     </row>
-    <row r="140" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="88"/>
       <c r="B140" s="88"/>
       <c r="C140" s="88"/>
@@ -7319,7 +7327,7 @@
       </c>
       <c r="T140" s="88"/>
     </row>
-    <row r="141" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="88"/>
       <c r="B141" s="88"/>
       <c r="C141" s="88"/>
@@ -7347,7 +7355,7 @@
       <c r="S141" s="85"/>
       <c r="T141" s="88"/>
     </row>
-    <row r="142" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="88"/>
       <c r="B142" s="88"/>
       <c r="C142" s="88"/>
@@ -7383,7 +7391,7 @@
       <c r="S142" s="88"/>
       <c r="T142" s="88"/>
     </row>
-    <row r="143" customFormat="false" ht="34.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="50" t="s">
         <v>575</v>
       </c>
@@ -7426,7 +7434,7 @@
       <c r="S143" s="88"/>
       <c r="T143" s="88"/>
     </row>
-    <row r="144" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="18" t="s">
         <v>586</v>
       </c>
@@ -7463,7 +7471,7 @@
       <c r="S144" s="88"/>
       <c r="T144" s="88"/>
     </row>
-    <row r="145" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="88"/>
       <c r="B145" s="88"/>
       <c r="C145" s="88"/>
@@ -7476,7 +7484,7 @@
       <c r="S145" s="88"/>
       <c r="T145" s="88"/>
     </row>
-    <row r="146" s="125" customFormat="true" ht="68.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" s="125" customFormat="true" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="116" t="s">
         <v>593</v>
       </c>
@@ -7516,7 +7524,7 @@
       <c r="S146" s="123"/>
       <c r="T146" s="123"/>
     </row>
-    <row r="147" s="125" customFormat="true" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" s="125" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="126" t="s">
         <v>602</v>
       </c>
@@ -7542,7 +7550,7 @@
       <c r="S147" s="123"/>
       <c r="T147" s="123"/>
     </row>
-    <row r="148" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="88"/>
       <c r="B148" s="88"/>
       <c r="C148" s="88"/>
@@ -7555,7 +7563,7 @@
       <c r="S148" s="88"/>
       <c r="T148" s="88"/>
     </row>
-    <row r="149" customFormat="false" ht="34.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="50" t="s">
         <v>604</v>
       </c>
@@ -7591,7 +7599,7 @@
       <c r="S149" s="88"/>
       <c r="T149" s="88"/>
     </row>
-    <row r="150" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="18" t="s">
         <v>612</v>
       </c>
@@ -7627,7 +7635,7 @@
       <c r="S150" s="88"/>
       <c r="T150" s="88"/>
     </row>
-    <row r="151" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="88"/>
       <c r="B151" s="88"/>
       <c r="C151" s="88"/>
@@ -7661,7 +7669,7 @@
       <c r="S151" s="88"/>
       <c r="T151" s="88"/>
     </row>
-    <row r="152" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="28"/>
       <c r="B152" s="8"/>
       <c r="C152" s="131"/>
@@ -7692,7 +7700,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="28"/>
       <c r="B153" s="8"/>
       <c r="C153" s="131"/>
@@ -7714,7 +7722,7 @@
       <c r="L153" s="3"/>
       <c r="M153" s="9"/>
     </row>
-    <row r="155" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E155" s="18" t="s">
         <v>634</v>
       </c>
@@ -7741,7 +7749,7 @@
       <c r="S155" s="95"/>
       <c r="T155" s="137"/>
     </row>
-    <row r="156" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E156" s="18" t="s">
         <v>634</v>
       </c>
@@ -7774,7 +7782,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E157" s="18"/>
       <c r="F157" s="18"/>
       <c r="G157" s="16"/>
@@ -7795,9 +7803,9 @@
       <c r="S157" s="81"/>
       <c r="T157" s="20"/>
     </row>
-    <row r="159" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E159" s="18"/>
-      <c r="F159" s="15" t="s">
+      <c r="F159" s="108" t="s">
         <v>28</v>
       </c>
       <c r="G159" s="16"/>
@@ -7825,7 +7833,7 @@
       <c r="S159" s="98"/>
       <c r="T159" s="137"/>
     </row>
-    <row r="160" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E160" s="18" t="s">
         <v>646</v>
       </c>
@@ -7862,7 +7870,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E161" s="18" t="s">
         <v>646</v>
       </c>
@@ -7889,7 +7897,7 @@
       <c r="R161" s="106"/>
       <c r="S161" s="98"/>
     </row>
-    <row r="162" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E162" s="18" t="s">
         <v>655</v>
       </c>
@@ -7914,7 +7922,7 @@
       <c r="R162" s="106"/>
       <c r="S162" s="98"/>
     </row>
-    <row r="164" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E164" s="18" t="s">
         <v>658</v>
       </c>
@@ -7943,7 +7951,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E165" s="18"/>
       <c r="F165" s="18"/>
       <c r="G165" s="16"/>
@@ -7960,7 +7968,7 @@
       <c r="N165" s="20"/>
       <c r="O165" s="20"/>
     </row>
-    <row r="167" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E167" s="18" t="s">
         <v>658</v>
       </c>
@@ -7994,7 +8002,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E170" s="18" t="s">
         <v>634</v>
       </c>
@@ -8028,7 +8036,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="2"/>
       <c r="B172" s="17"/>
       <c r="C172" s="29"/>
@@ -8059,7 +8067,7 @@
       </c>
       <c r="O172" s="18"/>
     </row>
-    <row r="173" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="2"/>
       <c r="B173" s="17"/>
       <c r="C173" s="29"/>
@@ -8105,8 +8113,7 @@
       <c r="N174" s="20"/>
       <c r="O174" s="18"/>
     </row>
-    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="176" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="2"/>
       <c r="B176" s="17"/>
       <c r="C176" s="29"/>
@@ -8139,7 +8146,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="2"/>
       <c r="B177" s="17"/>
       <c r="C177" s="29"/>
@@ -8164,7 +8171,7 @@
       <c r="N177" s="20"/>
       <c r="O177" s="144"/>
     </row>
-    <row r="178" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="2"/>
       <c r="B178" s="17"/>
       <c r="C178" s="29"/>
@@ -8185,31 +8192,31 @@
       <c r="N178" s="20"/>
       <c r="O178" s="20"/>
     </row>
-    <row r="179" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E179" s="14" t="s">
         <v>686</v>
       </c>
-      <c r="F179" s="58" t="s">
+      <c r="F179" s="145" t="s">
         <v>28</v>
       </c>
       <c r="G179" s="16"/>
       <c r="H179" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="Q179" s="145" t="s">
+      <c r="Q179" s="146" t="s">
         <v>687</v>
       </c>
       <c r="R179" s="106" t="s">
         <v>29</v>
       </c>
-      <c r="S179" s="146"/>
-      <c r="T179" s="147"/>
-    </row>
-    <row r="180" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S179" s="147"/>
+      <c r="T179" s="148"/>
+    </row>
+    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E180" s="14" t="s">
         <v>686</v>
       </c>
-      <c r="F180" s="148" t="s">
+      <c r="F180" s="145" t="s">
         <v>688</v>
       </c>
       <c r="G180" s="16" t="s">
@@ -8218,9 +8225,7 @@
       <c r="H180" s="17" t="s">
         <v>688</v>
       </c>
-      <c r="I180" s="18" t="s">
-        <v>690</v>
-      </c>
+      <c r="I180" s="0"/>
       <c r="J180" s="18"/>
       <c r="K180" s="18"/>
       <c r="L180" s="149" t="s">
@@ -8232,33 +8237,33 @@
       <c r="N180" s="95"/>
       <c r="O180" s="95"/>
       <c r="P180" s="98"/>
-      <c r="Q180" s="145" t="s">
+      <c r="Q180" s="146" t="s">
+        <v>690</v>
+      </c>
+      <c r="R180" s="106" t="s">
         <v>691</v>
       </c>
-      <c r="R180" s="106" t="s">
+      <c r="S180" s="150" t="s">
         <v>692</v>
       </c>
-      <c r="S180" s="150" t="s">
+      <c r="T180" s="45" t="s">
         <v>693</v>
       </c>
-      <c r="T180" s="45" t="s">
+    </row>
+    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E181" s="14" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="181" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E181" s="14" t="s">
+      <c r="F181" s="145" t="s">
+        <v>256</v>
+      </c>
+      <c r="G181" s="16" t="s">
         <v>695</v>
-      </c>
-      <c r="F181" s="148" t="s">
-        <v>256</v>
-      </c>
-      <c r="G181" s="16" t="s">
-        <v>696</v>
       </c>
       <c r="H181" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="I181" s="18"/>
+      <c r="I181" s="0"/>
       <c r="J181" s="18"/>
       <c r="K181" s="18"/>
       <c r="L181" s="149"/>
@@ -8266,29 +8271,31 @@
       <c r="N181" s="95"/>
       <c r="O181" s="95"/>
       <c r="P181" s="98"/>
-      <c r="Q181" s="145" t="s">
+      <c r="Q181" s="146" t="s">
+        <v>696</v>
+      </c>
+      <c r="R181" s="106" t="s">
         <v>697</v>
       </c>
-      <c r="R181" s="106" t="s">
+      <c r="S181" s="147"/>
+      <c r="T181" s="151"/>
+    </row>
+    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E182" s="14" t="s">
+        <v>694</v>
+      </c>
+      <c r="F182" s="145" t="s">
         <v>698</v>
       </c>
-      <c r="S181" s="146"/>
-      <c r="T181" s="151"/>
-    </row>
-    <row r="182" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E182" s="14" t="s">
+      <c r="G182" s="16" t="s">
         <v>695</v>
       </c>
-      <c r="F182" s="148" t="s">
+      <c r="H182" s="17" t="s">
+        <v>698</v>
+      </c>
+      <c r="I182" s="18" t="s">
         <v>699</v>
       </c>
-      <c r="G182" s="16" t="s">
-        <v>696</v>
-      </c>
-      <c r="H182" s="17" t="s">
-        <v>699</v>
-      </c>
-      <c r="I182" s="18"/>
       <c r="J182" s="18"/>
       <c r="K182" s="18"/>
       <c r="L182" s="149"/>
@@ -8298,18 +8305,18 @@
       <c r="P182" s="98"/>
       <c r="Q182" s="98"/>
       <c r="R182" s="106"/>
-      <c r="S182" s="146"/>
+      <c r="S182" s="147"/>
       <c r="T182" s="151"/>
     </row>
-    <row r="183" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E183" s="14" t="s">
+        <v>694</v>
+      </c>
+      <c r="F183" s="145" t="s">
+        <v>700</v>
+      </c>
+      <c r="G183" s="16" t="s">
         <v>695</v>
-      </c>
-      <c r="F183" s="148" t="s">
-        <v>700</v>
-      </c>
-      <c r="G183" s="16" t="s">
-        <v>696</v>
       </c>
       <c r="H183" s="17" t="s">
         <v>206</v>
@@ -8324,10 +8331,10 @@
       <c r="P183" s="152"/>
       <c r="Q183" s="152"/>
       <c r="R183" s="106"/>
-      <c r="S183" s="146"/>
+      <c r="S183" s="147"/>
       <c r="T183" s="151"/>
     </row>
-    <row r="185" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E185" s="18" t="s">
         <v>701</v>
       </c>
@@ -8362,7 +8369,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E186" s="18" t="s">
         <v>701</v>
       </c>
@@ -8385,7 +8392,7 @@
       <c r="Q186" s="45"/>
       <c r="R186" s="138"/>
     </row>
-    <row r="187" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E187" s="18" t="s">
         <v>708</v>
       </c>
@@ -8408,7 +8415,7 @@
       <c r="Q187" s="45"/>
       <c r="R187" s="138"/>
     </row>
-    <row r="189" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E189" s="18" t="s">
         <v>712</v>
       </c>
@@ -8433,7 +8440,7 @@
       <c r="N189" s="20"/>
       <c r="O189" s="20"/>
       <c r="P189" s="3"/>
-      <c r="Q189" s="145" t="s">
+      <c r="Q189" s="146" t="s">
         <v>716</v>
       </c>
       <c r="R189" s="106" t="s">
@@ -8443,7 +8450,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E190" s="18" t="s">
         <v>719</v>
       </c>
@@ -8464,7 +8471,7 @@
       <c r="N190" s="20"/>
       <c r="O190" s="20"/>
       <c r="P190" s="3"/>
-      <c r="Q190" s="145" t="s">
+      <c r="Q190" s="146" t="s">
         <v>722</v>
       </c>
       <c r="R190" s="106" t="s">
@@ -8472,7 +8479,7 @@
       </c>
       <c r="S190" s="98"/>
     </row>
-    <row r="191" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E191" s="18" t="s">
         <v>724</v>
       </c>
@@ -8497,7 +8504,7 @@
       <c r="R191" s="106"/>
       <c r="S191" s="98"/>
     </row>
-    <row r="193" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E193" s="18" t="s">
         <v>727</v>
       </c>
@@ -8522,7 +8529,7 @@
       <c r="N193" s="20"/>
       <c r="O193" s="20"/>
       <c r="P193" s="3"/>
-      <c r="Q193" s="145" t="s">
+      <c r="Q193" s="146" t="s">
         <v>731</v>
       </c>
       <c r="R193" s="106" t="s">
@@ -8532,7 +8539,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E194" s="18"/>
       <c r="F194" s="18"/>
       <c r="G194" s="16"/>
@@ -8545,7 +8552,7 @@
       <c r="N194" s="20"/>
       <c r="O194" s="20"/>
       <c r="P194" s="3"/>
-      <c r="Q194" s="145" t="s">
+      <c r="Q194" s="146" t="s">
         <v>734</v>
       </c>
       <c r="R194" s="106" t="s">
@@ -8553,7 +8560,7 @@
       </c>
       <c r="S194" s="98"/>
     </row>
-    <row r="195" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E195" s="18"/>
       <c r="F195" s="18"/>
       <c r="G195" s="16"/>
@@ -8566,7 +8573,7 @@
       <c r="N195" s="20"/>
       <c r="O195" s="20"/>
       <c r="P195" s="3"/>
-      <c r="Q195" s="145" t="s">
+      <c r="Q195" s="146" t="s">
         <v>736</v>
       </c>
       <c r="R195" s="106" t="s">
@@ -8574,7 +8581,7 @@
       </c>
       <c r="S195" s="98"/>
     </row>
-    <row r="197" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E197" s="14" t="s">
         <v>738</v>
       </c>
@@ -8601,7 +8608,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E198" s="14" t="s">
         <v>738</v>
       </c>
@@ -8620,7 +8627,7 @@
       <c r="L198" s="3"/>
       <c r="M198" s="76"/>
     </row>
-    <row r="199" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E199" s="14" t="s">
         <v>738</v>
       </c>
@@ -8639,7 +8646,7 @@
       <c r="L199" s="3"/>
       <c r="M199" s="76"/>
     </row>
-    <row r="201" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E201" s="18" t="s">
         <v>745</v>
       </c>
@@ -8667,7 +8674,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E202" s="18" t="s">
         <v>745</v>
       </c>
@@ -8691,7 +8698,7 @@
       </c>
       <c r="N202" s="115"/>
     </row>
-    <row r="203" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E203" s="18" t="s">
         <v>755</v>
       </c>
@@ -8715,7 +8722,7 @@
       </c>
       <c r="N203" s="20"/>
     </row>
-    <row r="204" customFormat="false" ht="17.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E204" s="18"/>
       <c r="F204" s="18"/>
       <c r="G204" s="16"/>
@@ -8732,17 +8739,6 @@
       <c r="N204" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="C152:D152"/>
-    <mergeCell ref="J152:K152"/>
-    <mergeCell ref="C153:D153"/>
-    <mergeCell ref="J153:K153"/>
-    <mergeCell ref="P183:Q183"/>
-    <mergeCell ref="O185:P185"/>
-    <mergeCell ref="O186:P186"/>
-    <mergeCell ref="O187:P187"/>
-    <mergeCell ref="P191:Q191"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>